<commit_message>
findings in test-suite Fixes #314
</commit_message>
<xml_diff>
--- a/testing/ApplicationPattern+testcase.docs.xlsx
+++ b/testing/ApplicationPattern+testcase.docs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IS00759329\Desktop\Telefonica\ApplicationPattern\ApplicationPattern_v2\testSuites_docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IS00759329\Desktop\Telefonica\ApplicationPattern\ApplicationPattern_v2\ApplicationLayerTopology\ApplicationLayerTopology-3\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B9FAB4-FABB-422C-857C-F63035A9D20D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18FA36A-BB17-4722-8D4B-39EADD8BFC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="285" yWindow="270" windowWidth="20205" windowHeight="10650" xr2:uid="{5947114D-DBB0-48EC-8A07-3C785D0D3740}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3739" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3740" uniqueCount="435">
   <si>
     <t>Registry Office</t>
   </si>
@@ -1935,6 +1935,14 @@
   <si>
     <t>#### Clearing:
 - PUT chosen op-c/op-s opertion-name with initial value</t>
+  </si>
+  <si>
+    <t>#### Clearing:
+- PUT initial newRelease/application-name
+- PUT initial newRelease/release-number
+- PUT initial newRelease/protocol
+- PUT initial newRelease/address
+- PUT initial newRelease/port</t>
   </si>
 </sst>
 </file>
@@ -2607,22 +2615,22 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2943,7 +2951,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2954,10 +2962,10 @@
   <dimension ref="A1:R282"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="K253" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B175" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M68" sqref="M68:M258"/>
+      <selection pane="bottomRight" activeCell="D177" sqref="D177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3140,7 +3148,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="112" t="s">
+      <c r="A4" s="115" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="13" t="s">
@@ -3212,7 +3220,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" ht="315" x14ac:dyDescent="0.25">
-      <c r="A5" s="112"/>
+      <c r="A5" s="115"/>
       <c r="B5" s="16" t="s">
         <v>22</v>
       </c>
@@ -3471,7 +3479,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="112"/>
+      <c r="A6" s="115"/>
       <c r="B6" s="16" t="s">
         <v>23</v>
       </c>
@@ -3561,7 +3569,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="112"/>
+      <c r="A7" s="115"/>
       <c r="B7" s="22" t="s">
         <v>26</v>
       </c>
@@ -3647,7 +3655,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="112" t="s">
+      <c r="A8" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="25" t="s">
@@ -3719,7 +3727,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" ht="285" x14ac:dyDescent="0.25">
-      <c r="A9" s="112"/>
+      <c r="A9" s="115"/>
       <c r="B9" s="26" t="s">
         <v>29</v>
       </c>
@@ -3899,7 +3907,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="112"/>
+      <c r="A10" s="115"/>
       <c r="B10" s="26" t="s">
         <v>30</v>
       </c>
@@ -3985,7 +3993,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="112"/>
+      <c r="A11" s="115"/>
       <c r="B11" s="22" t="str">
         <f t="shared" ref="B11:R11" si="7">$B7</f>
         <v>#### Clearing:
@@ -4073,7 +4081,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="112" t="s">
+      <c r="A12" s="115" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="25" t="s">
@@ -4145,7 +4153,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" ht="270" x14ac:dyDescent="0.25">
-      <c r="A13" s="114"/>
+      <c r="A13" s="117"/>
       <c r="B13" s="26" t="s">
         <v>33</v>
       </c>
@@ -4325,7 +4333,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="114"/>
+      <c r="A14" s="117"/>
       <c r="B14" s="26" t="s">
         <v>34</v>
       </c>
@@ -4411,7 +4419,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="114"/>
+      <c r="A15" s="117"/>
       <c r="B15" s="22" t="str">
         <f t="shared" ref="B15:R15" si="11">$B7</f>
         <v>#### Clearing:
@@ -4499,7 +4507,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="112" t="s">
+      <c r="A16" s="115" t="s">
         <v>35</v>
       </c>
       <c r="B16" s="25" t="s">
@@ -4571,7 +4579,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" ht="285" x14ac:dyDescent="0.25">
-      <c r="A17" s="112"/>
+      <c r="A17" s="115"/>
       <c r="B17" s="26" t="s">
         <v>37</v>
       </c>
@@ -4749,7 +4757,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="112"/>
+      <c r="A18" s="115"/>
       <c r="B18" s="26" t="s">
         <v>34</v>
       </c>
@@ -4835,7 +4843,7 @@
       </c>
     </row>
     <row r="19" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="112"/>
+      <c r="A19" s="115"/>
       <c r="B19" s="22" t="str">
         <f t="shared" ref="B19:R19" si="15">$B7</f>
         <v>#### Clearing:
@@ -4923,7 +4931,7 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="112" t="s">
+      <c r="A20" s="115" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="25" t="s">
@@ -4995,7 +5003,7 @@
       </c>
     </row>
     <row r="21" spans="1:18" ht="285" x14ac:dyDescent="0.25">
-      <c r="A21" s="112"/>
+      <c r="A21" s="115"/>
       <c r="B21" s="26" t="s">
         <v>40</v>
       </c>
@@ -5173,7 +5181,7 @@
       </c>
     </row>
     <row r="22" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="112"/>
+      <c r="A22" s="115"/>
       <c r="B22" s="26" t="s">
         <v>34</v>
       </c>
@@ -5259,7 +5267,7 @@
       </c>
     </row>
     <row r="23" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="112"/>
+      <c r="A23" s="115"/>
       <c r="B23" s="22" t="str">
         <f t="shared" ref="B23:R23" si="19">$B7</f>
         <v>#### Clearing:
@@ -5347,7 +5355,7 @@
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="112" t="s">
+      <c r="A24" s="115" t="s">
         <v>41</v>
       </c>
       <c r="B24" s="25" t="s">
@@ -5419,7 +5427,7 @@
       </c>
     </row>
     <row r="25" spans="1:18" ht="270" x14ac:dyDescent="0.25">
-      <c r="A25" s="112"/>
+      <c r="A25" s="115"/>
       <c r="B25" s="26" t="s">
         <v>43</v>
       </c>
@@ -5563,7 +5571,7 @@
       </c>
     </row>
     <row r="26" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="112"/>
+      <c r="A26" s="115"/>
       <c r="B26" s="26" t="s">
         <v>45</v>
       </c>
@@ -5639,7 +5647,7 @@
       </c>
     </row>
     <row r="27" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="112"/>
+      <c r="A27" s="115"/>
       <c r="B27" s="22" t="str">
         <f t="shared" ref="B27:M27" si="23">$B7</f>
         <v>#### Clearing:
@@ -5717,7 +5725,7 @@
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="112" t="s">
+      <c r="A28" s="115" t="s">
         <v>46</v>
       </c>
       <c r="B28" s="25" t="s">
@@ -5789,7 +5797,7 @@
       </c>
     </row>
     <row r="29" spans="1:18" ht="270" x14ac:dyDescent="0.25">
-      <c r="A29" s="112"/>
+      <c r="A29" s="115"/>
       <c r="B29" s="26" t="s">
         <v>48</v>
       </c>
@@ -5933,7 +5941,7 @@
       </c>
     </row>
     <row r="30" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="112"/>
+      <c r="A30" s="115"/>
       <c r="B30" s="26" t="s">
         <v>45</v>
       </c>
@@ -6009,7 +6017,7 @@
       </c>
     </row>
     <row r="31" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="112"/>
+      <c r="A31" s="115"/>
       <c r="B31" s="22" t="str">
         <f t="shared" ref="B31:M31" si="27">$B7</f>
         <v>#### Clearing:
@@ -6087,7 +6095,7 @@
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="112" t="s">
+      <c r="A32" s="115" t="s">
         <v>49</v>
       </c>
       <c r="B32" s="25" t="s">
@@ -6159,7 +6167,7 @@
       </c>
     </row>
     <row r="33" spans="1:18" ht="255" x14ac:dyDescent="0.25">
-      <c r="A33" s="112"/>
+      <c r="A33" s="115"/>
       <c r="B33" s="26" t="s">
         <v>51</v>
       </c>
@@ -6320,7 +6328,7 @@
       </c>
     </row>
     <row r="34" spans="1:18" ht="75" x14ac:dyDescent="0.25">
-      <c r="A34" s="112"/>
+      <c r="A34" s="115"/>
       <c r="B34" s="26" t="s">
         <v>52</v>
       </c>
@@ -6416,7 +6424,7 @@
       </c>
     </row>
     <row r="35" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="112"/>
+      <c r="A35" s="115"/>
       <c r="B35" s="22" t="str">
         <f t="shared" ref="B35:R35" si="31">$B7</f>
         <v>#### Clearing:
@@ -6504,7 +6512,7 @@
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="112" t="s">
+      <c r="A36" s="115" t="s">
         <v>55</v>
       </c>
       <c r="B36" s="25" t="s">
@@ -6576,7 +6584,7 @@
       </c>
     </row>
     <row r="37" spans="1:18" ht="255" x14ac:dyDescent="0.25">
-      <c r="A37" s="112"/>
+      <c r="A37" s="115"/>
       <c r="B37" s="26" t="s">
         <v>51</v>
       </c>
@@ -6732,7 +6740,7 @@
       </c>
     </row>
     <row r="38" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="112"/>
+      <c r="A38" s="115"/>
       <c r="B38" s="26" t="s">
         <v>57</v>
       </c>
@@ -6828,7 +6836,7 @@
       </c>
     </row>
     <row r="39" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="112"/>
+      <c r="A39" s="115"/>
       <c r="B39" s="22" t="str">
         <f t="shared" ref="B39:R39" si="35">$B7</f>
         <v>#### Clearing:
@@ -6916,7 +6924,7 @@
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="112" t="s">
+      <c r="A40" s="115" t="s">
         <v>60</v>
       </c>
       <c r="B40" s="25" t="s">
@@ -7354,7 +7362,7 @@
       </c>
     </row>
     <row r="44" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="112" t="s">
+      <c r="A44" s="115" t="s">
         <v>63</v>
       </c>
       <c r="B44" s="25" t="s">
@@ -8058,7 +8066,7 @@
       </c>
     </row>
     <row r="50" spans="1:18" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="112" t="s">
+      <c r="A50" s="115" t="s">
         <v>71</v>
       </c>
       <c r="B50" s="49" t="s">
@@ -8344,7 +8352,7 @@
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A54" s="116" t="s">
+      <c r="A54" s="114" t="s">
         <v>76</v>
       </c>
       <c r="B54" s="49" t="s">
@@ -8400,7 +8408,7 @@
       </c>
     </row>
     <row r="55" spans="1:18" ht="330" x14ac:dyDescent="0.25">
-      <c r="A55" s="116"/>
+      <c r="A55" s="114"/>
       <c r="B55" s="52" t="s">
         <v>78</v>
       </c>
@@ -8519,7 +8527,7 @@
       </c>
     </row>
     <row r="56" spans="1:18" ht="75" x14ac:dyDescent="0.25">
-      <c r="A56" s="116"/>
+      <c r="A56" s="114"/>
       <c r="B56" s="56" t="s">
         <v>79</v>
       </c>
@@ -8573,7 +8581,7 @@
       </c>
     </row>
     <row r="57" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="116"/>
+      <c r="A57" s="114"/>
       <c r="B57" s="57" t="s">
         <v>75</v>
       </c>
@@ -8683,7 +8691,7 @@
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A59" s="112" t="s">
+      <c r="A59" s="115" t="s">
         <v>83</v>
       </c>
       <c r="B59" s="25" t="s">
@@ -9073,7 +9081,7 @@
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A63" s="112" t="s">
+      <c r="A63" s="115" t="s">
         <v>89</v>
       </c>
       <c r="B63" s="25" t="s">
@@ -9145,7 +9153,7 @@
       </c>
     </row>
     <row r="64" spans="1:18" ht="270" x14ac:dyDescent="0.25">
-      <c r="A64" s="112"/>
+      <c r="A64" s="115"/>
       <c r="B64" s="26" t="s">
         <v>91</v>
       </c>
@@ -9295,7 +9303,7 @@
       </c>
     </row>
     <row r="65" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="112"/>
+      <c r="A65" s="115"/>
       <c r="B65" s="26" t="s">
         <v>92</v>
       </c>
@@ -9367,7 +9375,7 @@
       </c>
     </row>
     <row r="66" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="112"/>
+      <c r="A66" s="115"/>
       <c r="B66" s="62" t="s">
         <v>75</v>
       </c>
@@ -9441,7 +9449,7 @@
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A67" s="112" t="s">
+      <c r="A67" s="115" t="s">
         <v>93</v>
       </c>
       <c r="B67" s="25" t="s">
@@ -9513,7 +9521,7 @@
       </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A68" s="112"/>
+      <c r="A68" s="115"/>
       <c r="B68" s="25"/>
       <c r="C68" s="25" t="s">
         <v>244</v>
@@ -11860,7 +11868,7 @@
       <c r="R115" s="54"/>
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A116" s="112" t="s">
+      <c r="A116" s="115" t="s">
         <v>96</v>
       </c>
       <c r="B116" s="25" t="s">
@@ -11931,7 +11939,7 @@
       </c>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A117" s="112"/>
+      <c r="A117" s="115"/>
       <c r="B117" s="25"/>
       <c r="C117" s="14" t="s">
         <v>233</v>
@@ -14194,7 +14202,7 @@
       <c r="R171" s="21"/>
     </row>
     <row r="172" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A172" s="112" t="s">
+      <c r="A172" s="115" t="s">
         <v>105</v>
       </c>
       <c r="B172" s="25" t="s">
@@ -14250,7 +14258,7 @@
       </c>
     </row>
     <row r="173" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A173" s="112"/>
+      <c r="A173" s="115"/>
       <c r="B173" s="52" t="s">
         <v>191</v>
       </c>
@@ -14531,7 +14539,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="177" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:18" ht="90" x14ac:dyDescent="0.25">
       <c r="A177" s="113"/>
       <c r="B177" s="16" t="str">
         <f>$B7</f>
@@ -14543,10 +14551,8 @@
         <v>#### Clearing:
 - not applicable</v>
       </c>
-      <c r="D177" s="19" t="str">
-        <f>$B7</f>
-        <v>#### Clearing:
-- not applicable</v>
+      <c r="D177" s="19" t="s">
+        <v>434</v>
       </c>
       <c r="E177" s="73" t="s">
         <v>44</v>
@@ -14592,7 +14598,7 @@
       </c>
     </row>
     <row r="178" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A178" s="112" t="s">
+      <c r="A178" s="115" t="s">
         <v>111</v>
       </c>
       <c r="B178" s="49" t="s">
@@ -14648,7 +14654,7 @@
       </c>
     </row>
     <row r="179" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A179" s="112"/>
+      <c r="A179" s="115"/>
       <c r="B179" s="56" t="s">
         <v>191</v>
       </c>
@@ -14702,7 +14708,7 @@
       </c>
     </row>
     <row r="180" spans="1:18" ht="345" x14ac:dyDescent="0.25">
-      <c r="A180" s="112"/>
+      <c r="A180" s="115"/>
       <c r="B180" s="52" t="s">
         <v>113</v>
       </c>
@@ -15258,7 +15264,7 @@
       </c>
     </row>
     <row r="189" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A189" s="112" t="s">
+      <c r="A189" s="115" t="s">
         <v>117</v>
       </c>
       <c r="B189" s="25" t="s">
@@ -15314,7 +15320,7 @@
       </c>
     </row>
     <row r="190" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A190" s="112"/>
+      <c r="A190" s="115"/>
       <c r="B190" s="25"/>
       <c r="C190" s="33" t="s">
         <v>233</v>
@@ -15350,7 +15356,7 @@
       <c r="R190" s="34"/>
     </row>
     <row r="191" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A191" s="117"/>
+      <c r="A191" s="116"/>
       <c r="B191" s="26" t="s">
         <v>67</v>
       </c>
@@ -15420,7 +15426,7 @@
       </c>
     </row>
     <row r="192" spans="1:18" ht="390" x14ac:dyDescent="0.25">
-      <c r="A192" s="117"/>
+      <c r="A192" s="116"/>
       <c r="B192" s="26" t="s">
         <v>119</v>
       </c>
@@ -15640,7 +15646,7 @@
       </c>
     </row>
     <row r="193" spans="1:18" ht="180" x14ac:dyDescent="0.25">
-      <c r="A193" s="117"/>
+      <c r="A193" s="116"/>
       <c r="B193" s="26" t="s">
         <v>120</v>
       </c>
@@ -15694,7 +15700,7 @@
       </c>
     </row>
     <row r="194" spans="1:18" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="117"/>
+      <c r="A194" s="116"/>
       <c r="B194" s="26" t="s">
         <v>75</v>
       </c>
@@ -15863,7 +15869,7 @@
 - ExecutionAndTraceLog server to operate</v>
       </c>
       <c r="I197" s="39" t="str">
-        <f t="shared" ref="H197:I197" si="80">$B$191</f>
+        <f t="shared" ref="I197" si="80">$B$191</f>
         <v>#### Requires:
 - ExecutionAndTraceLog server to operate</v>
       </c>
@@ -18444,7 +18450,7 @@
       <c r="R255" s="28"/>
     </row>
     <row r="256" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A256" s="115" t="s">
+      <c r="A256" s="112" t="s">
         <v>122</v>
       </c>
       <c r="B256" s="25" t="s">
@@ -18500,7 +18506,7 @@
       </c>
     </row>
     <row r="257" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A257" s="115"/>
+      <c r="A257" s="112"/>
       <c r="B257" s="26" t="s">
         <v>191</v>
       </c>
@@ -18826,7 +18832,7 @@
       </c>
     </row>
     <row r="263" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A263" s="115" t="s">
+      <c r="A263" s="112" t="s">
         <v>126</v>
       </c>
       <c r="B263" s="25" t="s">
@@ -18882,7 +18888,7 @@
       </c>
     </row>
     <row r="264" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A264" s="115"/>
+      <c r="A264" s="112"/>
       <c r="B264" s="26" t="s">
         <v>191</v>
       </c>
@@ -19208,7 +19214,7 @@
       </c>
     </row>
     <row r="270" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A270" s="115" t="s">
+      <c r="A270" s="112" t="s">
         <v>129</v>
       </c>
       <c r="B270" s="25" t="s">
@@ -19536,7 +19542,7 @@
       </c>
     </row>
     <row r="276" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A276" s="115" t="s">
+      <c r="A276" s="112" t="s">
         <v>132</v>
       </c>
       <c r="B276" s="25" t="s">
@@ -19592,7 +19598,7 @@
       </c>
     </row>
     <row r="277" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A277" s="115"/>
+      <c r="A277" s="112"/>
       <c r="B277" s="26" t="s">
         <v>66</v>
       </c>
@@ -19946,6 +19952,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A44:A48"/>
     <mergeCell ref="A276:A282"/>
     <mergeCell ref="A54:A57"/>
     <mergeCell ref="A59:A62"/>
@@ -19958,18 +19976,6 @@
     <mergeCell ref="A256:A261"/>
     <mergeCell ref="A263:A268"/>
     <mergeCell ref="A270:A274"/>
-    <mergeCell ref="A50:A53"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A44:A48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -20988,7 +20994,7 @@
       </c>
     </row>
     <row r="5" spans="1:83" x14ac:dyDescent="0.25">
-      <c r="A5" s="112" t="s">
+      <c r="A5" s="115" t="s">
         <v>41</v>
       </c>
       <c r="B5" s="25" t="s">
@@ -21239,7 +21245,7 @@
       </c>
     </row>
     <row r="6" spans="1:83" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="112"/>
+      <c r="A6" s="115"/>
       <c r="B6" s="26" t="s">
         <v>140</v>
       </c>
@@ -22026,7 +22032,7 @@
       </c>
     </row>
     <row r="7" spans="1:83" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="112"/>
+      <c r="A7" s="115"/>
       <c r="B7" s="26" t="s">
         <v>45</v>
       </c>
@@ -22848,7 +22854,7 @@
       </c>
     </row>
     <row r="9" spans="1:83" x14ac:dyDescent="0.25">
-      <c r="A9" s="112" t="s">
+      <c r="A9" s="115" t="s">
         <v>46</v>
       </c>
       <c r="B9" s="25" t="s">
@@ -23099,7 +23105,7 @@
       </c>
     </row>
     <row r="10" spans="1:83" ht="105" x14ac:dyDescent="0.25">
-      <c r="A10" s="112"/>
+      <c r="A10" s="115"/>
       <c r="B10" s="26" t="s">
         <v>153</v>
       </c>
@@ -23886,7 +23892,7 @@
       </c>
     </row>
     <row r="11" spans="1:83" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="112"/>
+      <c r="A11" s="115"/>
       <c r="B11" s="26" t="s">
         <v>45</v>
       </c>
@@ -27323,7 +27329,7 @@
       </c>
     </row>
     <row r="19" spans="1:83" ht="105" x14ac:dyDescent="0.25">
-      <c r="A19" s="112"/>
+      <c r="A19" s="115"/>
       <c r="B19" s="26" t="s">
         <v>147</v>
       </c>
@@ -28734,7 +28740,7 @@
       <c r="CE22" s="104"/>
     </row>
     <row r="23" spans="1:83" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="112" t="s">
+      <c r="A23" s="115" t="s">
         <v>71</v>
       </c>
       <c r="B23" s="49" t="s">
@@ -30159,7 +30165,7 @@
       </c>
     </row>
     <row r="27" spans="1:83" x14ac:dyDescent="0.25">
-      <c r="A27" s="115" t="s">
+      <c r="A27" s="112" t="s">
         <v>76</v>
       </c>
       <c r="B27" s="49" t="s">
@@ -30410,7 +30416,7 @@
       </c>
     </row>
     <row r="28" spans="1:83" ht="120" x14ac:dyDescent="0.25">
-      <c r="A28" s="115"/>
+      <c r="A28" s="112"/>
       <c r="B28" s="52" t="s">
         <v>149</v>
       </c>
@@ -30949,7 +30955,7 @@
       </c>
     </row>
     <row r="29" spans="1:83" ht="75" x14ac:dyDescent="0.25">
-      <c r="A29" s="115"/>
+      <c r="A29" s="112"/>
       <c r="B29" s="56" t="s">
         <v>79</v>
       </c>
@@ -31328,7 +31334,7 @@
       </c>
     </row>
     <row r="30" spans="1:83" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="115"/>
+      <c r="A30" s="112"/>
       <c r="B30" s="57" t="s">
         <v>75</v>
       </c>
@@ -32028,7 +32034,7 @@
       </c>
     </row>
     <row r="32" spans="1:83" x14ac:dyDescent="0.25">
-      <c r="A32" s="112" t="s">
+      <c r="A32" s="115" t="s">
         <v>89</v>
       </c>
       <c r="B32" s="25" t="s">
@@ -32279,7 +32285,7 @@
       </c>
     </row>
     <row r="33" spans="1:83" ht="90" x14ac:dyDescent="0.25">
-      <c r="A33" s="112"/>
+      <c r="A33" s="115"/>
       <c r="B33" s="26" t="s">
         <v>151</v>
       </c>
@@ -32803,7 +32809,7 @@
       </c>
     </row>
     <row r="34" spans="1:83" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="112"/>
+      <c r="A34" s="115"/>
       <c r="B34" s="26" t="s">
         <v>92</v>
       </c>
@@ -33127,7 +33133,7 @@
       </c>
     </row>
     <row r="35" spans="1:83" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="112"/>
+      <c r="A35" s="115"/>
       <c r="B35" s="62" t="s">
         <v>75</v>
       </c>
@@ -33451,7 +33457,7 @@
       </c>
     </row>
     <row r="36" spans="1:83" x14ac:dyDescent="0.25">
-      <c r="A36" s="112" t="s">
+      <c r="A36" s="115" t="s">
         <v>93</v>
       </c>
       <c r="B36" s="25" t="s">
@@ -33702,7 +33708,7 @@
       </c>
     </row>
     <row r="37" spans="1:83" ht="105" x14ac:dyDescent="0.25">
-      <c r="A37" s="112"/>
+      <c r="A37" s="115"/>
       <c r="B37" s="26" t="s">
         <v>152</v>
       </c>
@@ -34138,7 +34144,7 @@
       </c>
     </row>
     <row r="38" spans="1:83" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="112"/>
+      <c r="A38" s="115"/>
       <c r="B38" s="26" t="s">
         <v>92</v>
       </c>
@@ -34387,7 +34393,7 @@
       </c>
     </row>
     <row r="39" spans="1:83" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="112"/>
+      <c r="A39" s="115"/>
       <c r="B39" s="62" t="str">
         <f>$B8</f>
         <v>#### Clearing:
@@ -34933,12 +34939,12 @@
       <c r="A126" s="80"/>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="115" t="s">
+      <c r="A127" s="112" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" s="115"/>
+      <c r="A128" s="112"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="113"/>
@@ -34953,12 +34959,12 @@
       <c r="A132" s="113"/>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="115" t="s">
+      <c r="A133" s="112" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="115"/>
+      <c r="A134" s="112"/>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="113"/>
@@ -34973,7 +34979,7 @@
       <c r="A138" s="113"/>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="115" t="s">
+      <c r="A139" s="112" t="s">
         <v>129</v>
       </c>
     </row>
@@ -34990,12 +34996,12 @@
       <c r="A143" s="113"/>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" s="115" t="s">
+      <c r="A144" s="112" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="115"/>
+      <c r="A145" s="112"/>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="113"/>

</xml_diff>